<commit_message>
Update all feature to excel form
</commit_message>
<xml_diff>
--- a/ProgramStudy/前期最終課題実装内容.xlsx
+++ b/ProgramStudy/前期最終課題実装内容.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20357"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A406B445-D589-4717-9022-13CE8C8ACB2D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C4ABD21-0E4E-40AC-9070-6C643C60DEE1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="35">
   <si>
     <t>サンプル</t>
     <phoneticPr fontId="1"/>
@@ -401,11 +401,30 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>EX</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>〇</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Animator State Machine (Unity Like)</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>×　(静的)</t>
+    <rPh sb="3" eb="5">
+      <t>セイテキ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>パラメーターはエントリーやステート間の移動の条件として機能します</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>それぞれのステートには、そのステートから別のステートに移行するためのトランジション・パラメータがあります</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>各ステートの各トランジションのトリガーとなる条件を設定可能</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -760,8 +779,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:C38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.45"/>
@@ -845,7 +864,7 @@
         <v>13</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="12" spans="2:3" x14ac:dyDescent="0.45">
@@ -853,7 +872,7 @@
         <v>14</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="13" spans="2:3" x14ac:dyDescent="0.45">
@@ -861,7 +880,7 @@
         <v>15</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="14" spans="2:3" x14ac:dyDescent="0.45">
@@ -869,7 +888,7 @@
         <v>16</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="16" spans="2:3" x14ac:dyDescent="0.45">
@@ -915,7 +934,7 @@
         <v>21</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="24" spans="2:3" x14ac:dyDescent="0.45">
@@ -923,7 +942,7 @@
         <v>22</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="26" spans="2:3" x14ac:dyDescent="0.45">
@@ -943,28 +962,32 @@
       <c r="B28" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C28" s="1"/>
+      <c r="C28" s="1" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="29" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B29" s="1" t="s">
         <v>25</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="30" spans="2:3" ht="36" x14ac:dyDescent="0.45">
       <c r="B30" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C30" s="1"/>
+      <c r="C30" s="1" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="31" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B31" s="1" t="s">
         <v>27</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="32" spans="2:3" x14ac:dyDescent="0.45">
@@ -972,12 +995,12 @@
         <v>28</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="34" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B34" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="35" spans="2:3" x14ac:dyDescent="0.45">
@@ -989,16 +1012,28 @@
       </c>
     </row>
     <row r="36" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B36" s="1"/>
-      <c r="C36" s="1"/>
-    </row>
-    <row r="37" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B37" s="1"/>
-      <c r="C37" s="1"/>
+      <c r="B36" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="37" spans="2:3" ht="36" x14ac:dyDescent="0.45">
+      <c r="B37" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="38" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B38" s="4"/>
-      <c r="C38" s="1"/>
+      <c r="B38" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>6</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>
@@ -1008,21 +1043,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="ドキュメント" ma:contentTypeID="0x010100981F00714534F248AF97D93A6B3CC418" ma:contentTypeVersion="7" ma:contentTypeDescription="新しいドキュメントを作成します。" ma:contentTypeScope="" ma:versionID="a212fa3ad4fca78dba78d07e15646a6c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="e822ce3d-65dd-42e4-9436-492eba98715f" xmlns:ns3="ee3fae6d-ee90-4c97-b168-7f59e8944755" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="d93d7569979febe116a9c04460b91276" ns2:_="" ns3:_="">
     <xsd:import namespace="e822ce3d-65dd-42e4-9436-492eba98715f"/>
@@ -1205,24 +1225,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6E62B27F-3B77-4EBC-BD2C-FA60B6F64B02}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0AC8CE91-577E-4356-A8E1-1C9EFD67022A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7F66C0D8-F136-4300-8409-155AF8DE3CEE}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1239,4 +1257,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0AC8CE91-577E-4356-A8E1-1C9EFD67022A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6E62B27F-3B77-4EBC-BD2C-FA60B6F64B02}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>